<commit_message>
solicitud grafica ajustada grado 9- guion 1
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado09/guion01/SolicitudGrafica_CS_09_01_CO_REC.xlsx
+++ b/fuentes/contenidos/grado09/guion01/SolicitudGrafica_CS_09_01_CO_REC.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="153">
   <si>
     <t>Asignatura:</t>
   </si>
@@ -520,6 +520,15 @@
     <t xml:space="preserve">Wiki commons
 File:Punch congo rubber cartoon.jpg
 </t>
+  </si>
+  <si>
+    <t>Fotografía</t>
+  </si>
+  <si>
+    <t>Vertical</t>
+  </si>
+  <si>
+    <t>FO1</t>
   </si>
 </sst>
 </file>
@@ -2239,9 +2248,9 @@
   <sheetPr codeName="Hoja1"/>
   <dimension ref="A1:P95"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="140" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="140" workbookViewId="0">
       <pane ySplit="9" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B13" sqref="B13"/>
+      <selection pane="bottomLeft" activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -2438,27 +2447,30 @@
       </c>
     </row>
     <row r="10" spans="1:16" s="12" customFormat="1" ht="54" x14ac:dyDescent="0.25">
-      <c r="A10" s="13" t="e">
-        <f>IF(OR(B10&lt;&gt;"",J10&lt;&gt;""),CONCATENATE(LEFT(#REF!,3),IF(MID(#REF!,4,2)+1&lt;10,CONCATENATE("0",MID(#REF!,4,2)+1))),"")</f>
-        <v>#REF!</v>
+      <c r="A10" s="13" t="s">
+        <v>152</v>
       </c>
       <c r="B10" s="26" t="s">
         <v>149</v>
       </c>
       <c r="C10" s="26"/>
-      <c r="D10" s="14"/>
-      <c r="E10" s="14"/>
-      <c r="F10" s="14" t="e">
+      <c r="D10" s="14" t="s">
+        <v>150</v>
+      </c>
+      <c r="E10" s="14" t="s">
+        <v>151</v>
+      </c>
+      <c r="F10" s="14" t="str">
         <f t="shared" ref="F10:F61" si="0">IF(OR(B10&lt;&gt;"",J10&lt;&gt;""),CONCATENATE($C$7,"_",$A10,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I10="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="G10" s="14" t="e">
+        <v>CS_09_01_CO_FO1n.png</v>
+      </c>
+      <c r="G10" s="14" t="str">
         <f>IF(F10&lt;&gt;"",IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,5,FALSE),IF($G$5="F1",'Definición técnica de imagenes'!$E$15,'Definición técnica de imagenes'!$F$13)),'Definición técnica de imagenes'!$E$16),"")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="H10" s="14" t="e">
+        <v>286 x 286 px</v>
+      </c>
+      <c r="H10" s="14" t="str">
         <f t="shared" ref="H10:H61" si="1">IF(I10&lt;&gt;"",IF(OR(B10&lt;&gt;"",J10&lt;&gt;""),CONCATENATE($C$7,"_",$A10,IF($G$4="Cuaderno de Estudio","_zoom",CONCATENATE("a",IF(LEFT($G$5,1)="F",".jpg",".png")))),""),"")</f>
-        <v>#REF!</v>
+        <v>CS_09_01_CO_FO1a.png</v>
       </c>
       <c r="I10" s="14" t="str">
         <f>IF(OR(B10&lt;&gt;"",J10&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>

</xml_diff>